<commit_message>
Deploying to gh-pages from @ torstees/ncpi-fhir-ig-2@2b72d2b266bcea7a680bf6dea3102a0846a80f3a 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-research-data-access-code.xlsx
+++ b/CodeSystem-research-data-access-code.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-11T22:11:27+00:00</t>
+    <t>2024-03-15T21:50:53+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -117,7 +117,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>9</t>
+    <t>10</t>
   </si>
   <si>
     <t>Level</t>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t>Genetic studies only</t>
+  </si>
+  <si>
+    <t>GSR</t>
+  </si>
+  <si>
+    <t>Genomic Summary Results</t>
   </si>
 </sst>
 </file>
@@ -491,7 +497,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -619,6 +625,18 @@
       </c>
       <c r="D10" s="2"/>
     </row>
+    <row r="11">
+      <c r="A11" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>